<commit_message>
Commit with validating sorting functionality of pricing bar and completing all the scenarios
</commit_message>
<xml_diff>
--- a/KonakartAutomation/src/test/resources/testData/testinput.xlsx
+++ b/KonakartAutomation/src/test/resources/testData/testinput.xlsx
@@ -4,11 +4,14 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="14265" windowHeight="4890" tabRatio="544"/>
+    <workbookView windowWidth="13740" windowHeight="4890" tabRatio="544" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="right products " sheetId="11" r:id="rId1"/>
     <sheet name="wrong products" sheetId="12" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="13" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="14" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="15" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
   <oleSize ref="A1:B1"/>
@@ -16,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
   <si>
     <t>Computer Peripherals</t>
   </si>
@@ -55,6 +58,27 @@
   </si>
   <si>
     <t>gywdcygvgy</t>
+  </si>
+  <si>
+    <t>graphics cards</t>
+  </si>
+  <si>
+    <t>No products were found for your search</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>120</t>
+  </si>
+  <si>
+    <t>150</t>
   </si>
 </sst>
 </file>
@@ -67,12 +91,32 @@
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -92,14 +136,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -108,9 +144,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -125,7 +183,29 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -138,23 +218,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -169,51 +250,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -235,13 +271,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -253,25 +307,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -283,13 +409,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -302,108 +440,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -420,6 +456,17 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -448,6 +495,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -462,28 +524,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -506,15 +551,6 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
@@ -525,7 +561,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -543,135 +579,144 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -995,8 +1040,8 @@
   <sheetPr/>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="2"/>
@@ -1062,7 +1107,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="2"/>
@@ -1098,4 +1143,115 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="22.4285714285714" customWidth="1"/>
+    <col min="2" max="2" width="14.7142857142857" customWidth="1"/>
+    <col min="3" max="3" width="55.4285714285714" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="$A1:$XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="22.4285714285714" customWidth="1"/>
+    <col min="2" max="2" width="14.2857142857143" customWidth="1"/>
+    <col min="3" max="3" width="17.4285714285714" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="4"/>
+  <cols>
+    <col min="1" max="1" width="12.8571428571429" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>